<commit_message>
Se actualizan circulares pendientes, y se repara circular.php ya que ahora la ASFI genera sus circulares en HTTPS para descarga.
</commit_message>
<xml_diff>
--- a/normativa/Anexos/L04T01C01/L04T01C01A07.xlsx
+++ b/normativa/Anexos/L04T01C01/L04T01C01A07.xlsx
@@ -5,26 +5,26 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KARINA ARANDA\Reglamento de protección del consumidor de servicios financieros\Modificaciones Jefatura Educacion Financiera\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\DNP\Protección del Consumidor de SF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Educación" sheetId="3" r:id="rId1"/>
     <sheet name="Información" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Educación!$A$1:$O$28</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Información!$A$1:$M$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Educación!$A$1:$O$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Información!$A$1:$M$30</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>N°</t>
   </si>
@@ -114,13 +114,25 @@
   </si>
   <si>
     <t>MEDIOS O CANALES DE DIFUSIÓN ESTABLECIDOS</t>
+  </si>
+  <si>
+    <t>Elaborado por:</t>
+  </si>
+  <si>
+    <t>Gerente General</t>
+  </si>
+  <si>
+    <t>La presente declaración jurada conlleva la condición de confesión, verdad y certeza jurídica, de conformidad con lo dispuesto en el Artículo 1322° del Código Civil y el Parágrafo IV del Artículo157° del Código Procesal Civil, sujeta en caso de inexactitud o falsedad a la cancelación del trámite y a las penalidades establecidas en el Artículo 169° del Código Penal como falso testimonio.</t>
+  </si>
+  <si>
+    <t>Responsable de la Ejecución del Programa de Educación Financiera</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +183,30 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -186,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -479,11 +515,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="39" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -540,18 +595,56 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="39" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,43 +654,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -618,21 +690,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="9" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_III" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -648,7 +721,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -937,13 +1010,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:N6"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5703125" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
@@ -956,63 +1029,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
@@ -1036,42 +1109,42 @@
       <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
     </row>
     <row r="7" spans="1:17" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
@@ -1089,46 +1162,46 @@
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33" t="s">
+      <c r="F8" s="30"/>
+      <c r="G8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33" t="s">
+      <c r="H8" s="30"/>
+      <c r="I8" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="36" t="s">
+      <c r="N8" s="33" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="32"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="19" t="s">
         <v>18</v>
       </c>
@@ -1141,198 +1214,198 @@
       <c r="H9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="37"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="34"/>
     </row>
     <row r="10" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="24">
+      <c r="B10" s="38">
         <v>1</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="21"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
     </row>
     <row r="11" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
     </row>
     <row r="12" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="15"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
     </row>
     <row r="13" spans="1:17" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="25"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="22"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
     </row>
     <row r="14" spans="1:17" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="24">
+      <c r="B14" s="38">
         <v>2</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="14"/>
-      <c r="F14" s="26"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="26"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="40"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
     </row>
     <row r="15" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="15"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
     </row>
     <row r="16" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="21"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
     </row>
     <row r="17" spans="2:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="25"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="16"/>
-      <c r="F17" s="22"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
     </row>
     <row r="18" spans="2:14" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="24">
+      <c r="B18" s="38">
         <v>3</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="26"/>
+      <c r="F18" s="40"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="26"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="40"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
     </row>
     <row r="19" spans="2:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="24"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="36"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
     </row>
     <row r="20" spans="2:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
       <c r="E20" s="15"/>
-      <c r="F20" s="21"/>
+      <c r="F20" s="36"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
     </row>
     <row r="21" spans="2:14" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="25"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="22"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
     </row>
     <row r="22" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
@@ -1348,19 +1421,22 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+    <row r="23" spans="2:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
@@ -1377,37 +1453,55 @@
       <c r="N24" s="1"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
       <c r="N26" s="12"/>
     </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C28" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C29" s="22"/>
+      <c r="D29" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="A1:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A5:O5"/>
-    <mergeCell ref="B6:N6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
+  <mergeCells count="42">
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="B23:N23"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="M18:M21"/>
+    <mergeCell ref="N18:N21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="J18:J21"/>
     <mergeCell ref="N14:N17"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="C10:C13"/>
@@ -1424,26 +1518,32 @@
     <mergeCell ref="N10:N13"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C14:C17"/>
-    <mergeCell ref="M18:M21"/>
-    <mergeCell ref="N18:N21"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="A1:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A5:O5"/>
+    <mergeCell ref="B6:N6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;L&amp;"Times New Roman,Normal"Control de versiones
-Circular ASFI/530/2018 (última) &amp;"-,Normal"
+Circular ASFI/667/2020 (última) &amp;"-,Regular"
 &amp;R&amp;"Times New Roman,Normal"Libro 4°
 Título I
 Capítulo I
 Anexo 7
-Página 1/2&amp;"-,Normal"
+Página 1/2&amp;"-,Regular"
 </oddFooter>
   </headerFooter>
 </worksheet>
@@ -1451,16 +1551,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E9"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" customWidth="1"/>
@@ -1476,59 +1573,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
       <c r="N1" s="3"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
       <c r="N2" s="3"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -1552,39 +1649,39 @@
       <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
       <c r="N5" s="5"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
@@ -1600,243 +1697,320 @@
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="48" t="s">
+      <c r="L8" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="47"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="49"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="46"/>
     </row>
     <row r="10" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="24">
+      <c r="B10" s="38">
         <v>1</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="40"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="47"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="40"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="47"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="25"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="41"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="48"/>
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:16" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="45">
+      <c r="B14" s="52">
         <v>2</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="51"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="20"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="35"/>
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="40"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="47"/>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="40"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="47"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="25"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="41"/>
+    <row r="17" spans="2:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="39"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="48"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="42">
+    <row r="18" spans="2:14" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="49">
         <v>3</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="44"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="20"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="35"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="24"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="40"/>
+    <row r="19" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="38"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="47"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="40"/>
+    <row r="20" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="38"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="47"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="25"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="41"/>
+    <row r="21" spans="2:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="39"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="48"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
+    <row r="22" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C28" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C29" s="22"/>
+      <c r="D29" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="M29" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="40">
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
     <mergeCell ref="L10:L13"/>
     <mergeCell ref="A1:M2"/>
     <mergeCell ref="A3:M3"/>
@@ -1853,38 +2027,17 @@
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="L18:L21"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="K10:K13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
   </mergeCells>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="47" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.11811023622047245" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;L&amp;"Times New Roman,Normal"Control de versiones
-Circular ASFI/530/2018 (última) &amp;"-,Normal"
+Circular ASFI/667/2020 (última) &amp;"-,Regular"
 &amp;R&amp;"Times New Roman,Normal"&amp;10Libro 4°
 &amp;11Título I
 Capítulo I
 Anexo 7
-Página 2/2&amp;"-,Normal"
+Página 2/2&amp;"-,Regular"
 </oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>